<commit_message>
added new independent candidates
</commit_message>
<xml_diff>
--- a/db_resources/candidate_tracker.xlsx
+++ b/db_resources/candidate_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\Documents\code\vaelects\db_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C8F84D-532D-4C4A-9CBF-CF46DB01FCA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AC27CA-C404-4861-864F-0BD5A6A33996}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="558">
   <si>
     <t>id</t>
   </si>
@@ -1695,6 +1695,24 @@
   </si>
   <si>
     <t>https://senatorbillcarrico.com/</t>
+  </si>
+  <si>
+    <t>Connie</t>
+  </si>
+  <si>
+    <t>Hutchinson</t>
+  </si>
+  <si>
+    <t>ind</t>
+  </si>
+  <si>
+    <t>http://www.conniehutchinson.com/</t>
+  </si>
+  <si>
+    <t>Linnard</t>
+  </si>
+  <si>
+    <t>Harris Jr</t>
   </si>
 </sst>
 </file>
@@ -2048,10 +2066,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J147"/>
+  <dimension ref="A1:J149"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5951,6 +5969,58 @@
       </c>
       <c r="J147">
         <v>3401</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>2111</v>
+      </c>
+      <c r="B148" t="s">
+        <v>552</v>
+      </c>
+      <c r="D148" t="s">
+        <v>553</v>
+      </c>
+      <c r="E148" t="s">
+        <v>555</v>
+      </c>
+      <c r="F148" t="s">
+        <v>554</v>
+      </c>
+      <c r="G148" t="s">
+        <v>14</v>
+      </c>
+      <c r="H148">
+        <v>86</v>
+      </c>
+      <c r="J148">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>2121</v>
+      </c>
+      <c r="B149" t="s">
+        <v>556</v>
+      </c>
+      <c r="C149" t="s">
+        <v>184</v>
+      </c>
+      <c r="D149" t="s">
+        <v>557</v>
+      </c>
+      <c r="F149" t="s">
+        <v>554</v>
+      </c>
+      <c r="G149" t="s">
+        <v>14</v>
+      </c>
+      <c r="H149">
+        <v>70</v>
+      </c>
+      <c r="J149">
+        <v>821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added three more vasenate candidates
</commit_message>
<xml_diff>
--- a/db_resources/candidate_tracker.xlsx
+++ b/db_resources/candidate_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\Documents\code\vaelects\db_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3983195D-B0F7-46D6-A762-7ACBBE2F3E71}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0109CDBC-E60D-4D42-8051-435C816FE257}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vahouse" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="572">
   <si>
     <t>id</t>
   </si>
@@ -1731,16 +1731,48 @@
   </si>
   <si>
     <t>http://www.delegaterandyminchew.com/</t>
+  </si>
+  <si>
+    <t>Wayne</t>
+  </si>
+  <si>
+    <t>Powell</t>
+  </si>
+  <si>
+    <t>Amy</t>
+  </si>
+  <si>
+    <t>Laufer</t>
+  </si>
+  <si>
+    <t>Geary</t>
+  </si>
+  <si>
+    <t>Higgins</t>
+  </si>
+  <si>
+    <t>https://www.powellsenateva.com/</t>
+  </si>
+  <si>
+    <t>https://www.lauferforvirginia.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1763,14 +1795,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2085,7 +2120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
@@ -6125,10 +6160,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7907,8 +7942,94 @@
         <v>2261</v>
       </c>
     </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>2161</v>
+      </c>
+      <c r="B63" t="s">
+        <v>564</v>
+      </c>
+      <c r="D63" t="s">
+        <v>565</v>
+      </c>
+      <c r="E63" t="s">
+        <v>570</v>
+      </c>
+      <c r="F63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G63" t="s">
+        <v>406</v>
+      </c>
+      <c r="H63">
+        <v>11</v>
+      </c>
+      <c r="I63" t="s">
+        <v>95</v>
+      </c>
+      <c r="J63">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>2171</v>
+      </c>
+      <c r="B64" t="s">
+        <v>566</v>
+      </c>
+      <c r="D64" t="s">
+        <v>567</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="F64" t="s">
+        <v>17</v>
+      </c>
+      <c r="G64" t="s">
+        <v>406</v>
+      </c>
+      <c r="H64">
+        <v>17</v>
+      </c>
+      <c r="I64" t="s">
+        <v>95</v>
+      </c>
+      <c r="J64">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>2181</v>
+      </c>
+      <c r="B65" t="s">
+        <v>568</v>
+      </c>
+      <c r="D65" t="s">
+        <v>569</v>
+      </c>
+      <c r="F65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" t="s">
+        <v>406</v>
+      </c>
+      <c r="H65">
+        <v>13</v>
+      </c>
+      <c r="I65" t="s">
+        <v>95</v>
+      </c>
+      <c r="J65">
+        <v>1781</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J62" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <hyperlinks>
+    <hyperlink ref="E64" r:id="rId1" xr:uid="{7D1DC84B-8DC4-4F66-BB50-F57DA37F974D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Karren Torrent, D-vasenate 35
</commit_message>
<xml_diff>
--- a/db_resources/candidate_tracker.xlsx
+++ b/db_resources/candidate_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\Documents\code\vaelects\db_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED384D4E-C5F0-4E51-B95B-2C8D019479CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B4B4D0-88FB-4877-A9B9-26A22BD0CD1E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9420" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="644">
   <si>
     <t>id</t>
   </si>
@@ -1965,6 +1965,12 @@
   </si>
   <si>
     <t>https://losifordelegate.com/</t>
+  </si>
+  <si>
+    <t>Karrent</t>
+  </si>
+  <si>
+    <t>Torrent</t>
   </si>
 </sst>
 </file>
@@ -7006,10 +7012,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K78"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9225,6 +9231,32 @@
       </c>
       <c r="K78">
         <v>1451</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>10311</v>
+      </c>
+      <c r="B79" t="s">
+        <v>642</v>
+      </c>
+      <c r="D79" t="s">
+        <v>643</v>
+      </c>
+      <c r="F79" t="s">
+        <v>20</v>
+      </c>
+      <c r="G79" t="s">
+        <v>442</v>
+      </c>
+      <c r="H79">
+        <v>35</v>
+      </c>
+      <c r="J79">
+        <v>1771</v>
+      </c>
+      <c r="K79">
+        <v>1471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kelly McGinne-D, vahouse 13
</commit_message>
<xml_diff>
--- a/db_resources/candidate_tracker.xlsx
+++ b/db_resources/candidate_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\Documents\code\vaelects\db_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B4B4D0-88FB-4877-A9B9-26A22BD0CD1E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA14E8DB-05A8-4F21-AB74-40C10A608619}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9420" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vahouse" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="645">
   <si>
     <t>id</t>
   </si>
@@ -1971,6 +1971,9 @@
   </si>
   <si>
     <t>Torrent</t>
+  </si>
+  <si>
+    <t>McGinn</t>
   </si>
 </sst>
 </file>
@@ -2401,10 +2404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K174"/>
+  <dimension ref="A1:K175"/>
   <sheetViews>
-    <sheetView topLeftCell="F149" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J165" activeCellId="1" sqref="A165:A174 J165:J174"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I169" sqref="I169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7003,6 +7006,29 @@
         <v>941</v>
       </c>
     </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B175" t="s">
+        <v>53</v>
+      </c>
+      <c r="D175" t="s">
+        <v>644</v>
+      </c>
+      <c r="F175" t="s">
+        <v>20</v>
+      </c>
+      <c r="G175" t="s">
+        <v>14</v>
+      </c>
+      <c r="H175">
+        <v>13</v>
+      </c>
+      <c r="J175">
+        <v>2881</v>
+      </c>
+      <c r="K175">
+        <v>251</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J148" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -7014,7 +7040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
M. Jones withdrew from race
</commit_message>
<xml_diff>
--- a/db_resources/candidate_tracker.xlsx
+++ b/db_resources/candidate_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\Documents\code\vaelects\db_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA14E8DB-05A8-4F21-AB74-40C10A608619}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9591911-7422-4AEA-80CD-26FB324AC84B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vahouse" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="646">
   <si>
     <t>id</t>
   </si>
@@ -1974,24 +1974,19 @@
   </si>
   <si>
     <t>McGinn</t>
+  </si>
+  <si>
+    <t>WITHDREW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -2014,16 +2009,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2406,8 +2398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I169" sqref="I169"/>
+    <sheetView topLeftCell="A159" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7007,6 +6999,9 @@
       </c>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>10321</v>
+      </c>
       <c r="B175" t="s">
         <v>53</v>
       </c>
@@ -7040,8 +7035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7645,10 +7640,7 @@
         <v>12</v>
       </c>
       <c r="I21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21">
-        <v>1741</v>
+        <v>645</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -8858,7 +8850,7 @@
       <c r="D64" t="s">
         <v>590</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" t="s">
         <v>591</v>
       </c>
       <c r="F64" t="s">
@@ -9286,9 +9278,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E64" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>